<commit_message>
- Updated RNG to be more random - Fixed some broken images - Fixed a bug where armour cards were never displayed.
</commit_message>
<xml_diff>
--- a/PVPlayTool/Data/DarkSouls/DaS_Weapons.xlsx
+++ b/PVPlayTool/Data/DarkSouls/DaS_Weapons.xlsx
@@ -301,9 +301,6 @@
     <t>Caestus</t>
   </si>
   <si>
-    <t>Claws</t>
-  </si>
-  <si>
     <t>Dragon Bone Fist</t>
   </si>
   <si>
@@ -847,9 +844,6 @@
     <t>tex_DaS_Caestus.png</t>
   </si>
   <si>
-    <t>tex_DaS_Claws.png</t>
-  </si>
-  <si>
     <t>tex_DaS_DragonBoneFist.png</t>
   </si>
   <si>
@@ -1145,6 +1139,12 @@
   </si>
   <si>
     <t>tex_DaS_ManserpentGreatsword.png</t>
+  </si>
+  <si>
+    <t>Claw</t>
+  </si>
+  <si>
+    <t>tex_DaS_Claw.png</t>
   </si>
 </sst>
 </file>
@@ -1561,8 +1561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="G85" sqref="G85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1595,7 +1595,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1618,7 +1618,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1641,7 +1641,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1664,7 +1664,7 @@
         <v>2</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1687,7 +1687,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1710,7 +1710,7 @@
         <v>3</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1733,7 +1733,7 @@
         <v>3</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1756,7 +1756,7 @@
         <v>3</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1779,7 +1779,7 @@
         <v>3</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1802,7 +1802,7 @@
         <v>0</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1825,7 +1825,7 @@
         <v>0</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1848,7 +1848,7 @@
         <v>0</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1871,7 +1871,7 @@
         <v>1</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1894,7 +1894,7 @@
         <v>1</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1917,7 +1917,7 @@
         <v>2</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1940,7 +1940,7 @@
         <v>2</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1963,7 +1963,7 @@
         <v>3</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1986,7 +1986,7 @@
         <v>3</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -2009,7 +2009,7 @@
         <v>2</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -2032,7 +2032,7 @@
         <v>1</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -2055,7 +2055,7 @@
         <v>0</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -2078,7 +2078,7 @@
         <v>2</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -2101,7 +2101,7 @@
         <v>1</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -2124,7 +2124,7 @@
         <v>2</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -2147,7 +2147,7 @@
         <v>2</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -2170,7 +2170,7 @@
         <v>1</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -2193,7 +2193,7 @@
         <v>3</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -2216,7 +2216,7 @@
         <v>3</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -2239,7 +2239,7 @@
         <v>3</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -2262,7 +2262,7 @@
         <v>3</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -2285,7 +2285,7 @@
         <v>2</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -2308,7 +2308,7 @@
         <v>3</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -2331,7 +2331,7 @@
         <v>3</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -2354,7 +2354,7 @@
         <v>3</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -2377,7 +2377,7 @@
         <v>0</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -2400,7 +2400,7 @@
         <v>2</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -2423,7 +2423,7 @@
         <v>1</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -2446,7 +2446,7 @@
         <v>2</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -2469,7 +2469,7 @@
         <v>1</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -2492,7 +2492,7 @@
         <v>2</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -2515,7 +2515,7 @@
         <v>2</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -2538,7 +2538,7 @@
         <v>3</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -2561,7 +2561,7 @@
         <v>2</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -2584,7 +2584,7 @@
         <v>1</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -2607,7 +2607,7 @@
         <v>3</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -2630,7 +2630,7 @@
         <v>1</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -2653,7 +2653,7 @@
         <v>1</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -2676,7 +2676,7 @@
         <v>0</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -2699,7 +2699,7 @@
         <v>3</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -2722,7 +2722,7 @@
         <v>0</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -2745,7 +2745,7 @@
         <v>2</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -2768,7 +2768,7 @@
         <v>3</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -2791,7 +2791,7 @@
         <v>0</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -2814,7 +2814,7 @@
         <v>1</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -2837,7 +2837,7 @@
         <v>0</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -2860,7 +2860,7 @@
         <v>3</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -2883,7 +2883,7 @@
         <v>2</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -2906,7 +2906,7 @@
         <v>0</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -2929,7 +2929,7 @@
         <v>1</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -2952,7 +2952,7 @@
         <v>0</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
@@ -2975,7 +2975,7 @@
         <v>1</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -2998,7 +2998,7 @@
         <v>1</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -3021,7 +3021,7 @@
         <v>2</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -3044,7 +3044,7 @@
         <v>2</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -3067,7 +3067,7 @@
         <v>1</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -3090,7 +3090,7 @@
         <v>3</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -3113,7 +3113,7 @@
         <v>3</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
@@ -3136,7 +3136,7 @@
         <v>2</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -3159,7 +3159,7 @@
         <v>0</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -3182,7 +3182,7 @@
         <v>1</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
@@ -3205,7 +3205,7 @@
         <v>0</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -3228,7 +3228,7 @@
         <v>1</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -3251,7 +3251,7 @@
         <v>1</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -3274,7 +3274,7 @@
         <v>1</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -3297,7 +3297,7 @@
         <v>2</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
@@ -3320,7 +3320,7 @@
         <v>2</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -3343,7 +3343,7 @@
         <v>2</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
@@ -3366,7 +3366,7 @@
         <v>2</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
@@ -3389,7 +3389,7 @@
         <v>1</v>
       </c>
       <c r="G79" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
@@ -3412,7 +3412,7 @@
         <v>2</v>
       </c>
       <c r="G80" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
@@ -3435,7 +3435,7 @@
         <v>3</v>
       </c>
       <c r="G81" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -3458,7 +3458,7 @@
         <v>3</v>
       </c>
       <c r="G82" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -3481,7 +3481,7 @@
         <v>1</v>
       </c>
       <c r="G83" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -3504,12 +3504,12 @@
         <v>0</v>
       </c>
       <c r="G84" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>89</v>
+        <v>369</v>
       </c>
       <c r="B85">
         <v>6</v>
@@ -3527,12 +3527,12 @@
         <v>1</v>
       </c>
       <c r="G85" s="2" t="s">
-        <v>271</v>
+        <v>370</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B86">
         <v>20</v>
@@ -3550,12 +3550,12 @@
         <v>2</v>
       </c>
       <c r="G86" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B87">
         <v>0</v>
@@ -3573,12 +3573,12 @@
         <v>3</v>
       </c>
       <c r="G87" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B88">
         <v>11</v>
@@ -3596,12 +3596,12 @@
         <v>0</v>
       </c>
       <c r="G88" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B89">
         <v>13</v>
@@ -3619,12 +3619,12 @@
         <v>1</v>
       </c>
       <c r="G89" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B90">
         <v>12</v>
@@ -3642,12 +3642,12 @@
         <v>2</v>
       </c>
       <c r="G90" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B91">
         <v>24</v>
@@ -3665,12 +3665,12 @@
         <v>1</v>
       </c>
       <c r="G91" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B92">
         <v>24</v>
@@ -3688,12 +3688,12 @@
         <v>3</v>
       </c>
       <c r="G92" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B93">
         <v>13</v>
@@ -3711,12 +3711,12 @@
         <v>1</v>
       </c>
       <c r="G93" s="2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B94">
         <v>16</v>
@@ -3734,12 +3734,12 @@
         <v>2</v>
       </c>
       <c r="G94" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B95">
         <v>16</v>
@@ -3757,12 +3757,12 @@
         <v>2</v>
       </c>
       <c r="G95" s="2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B96">
         <v>12</v>
@@ -3780,12 +3780,12 @@
         <v>2</v>
       </c>
       <c r="G96" s="2" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B97">
         <v>15</v>
@@ -3803,12 +3803,12 @@
         <v>3</v>
       </c>
       <c r="G97" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B98">
         <v>16</v>
@@ -3826,12 +3826,12 @@
         <v>0</v>
       </c>
       <c r="G98" s="2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B99">
         <v>16</v>
@@ -3849,12 +3849,12 @@
         <v>1</v>
       </c>
       <c r="G99" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B100">
         <v>16</v>
@@ -3872,12 +3872,12 @@
         <v>3</v>
       </c>
       <c r="G100" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B101">
         <v>32</v>
@@ -3895,12 +3895,12 @@
         <v>3</v>
       </c>
       <c r="G101" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B102">
         <v>14</v>
@@ -3918,12 +3918,12 @@
         <v>1</v>
       </c>
       <c r="G102" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B103">
         <v>16</v>
@@ -3941,12 +3941,12 @@
         <v>2</v>
       </c>
       <c r="G103" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B104">
         <v>14</v>
@@ -3964,12 +3964,12 @@
         <v>1</v>
       </c>
       <c r="G104" s="2" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B105">
         <v>15</v>
@@ -3987,12 +3987,12 @@
         <v>1</v>
       </c>
       <c r="G105" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B106">
         <v>36</v>
@@ -4010,12 +4010,12 @@
         <v>2</v>
       </c>
       <c r="G106" s="2" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B107">
         <v>7</v>
@@ -4033,12 +4033,12 @@
         <v>0</v>
       </c>
       <c r="G107" s="2" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B108">
         <v>8</v>
@@ -4056,12 +4056,12 @@
         <v>1</v>
       </c>
       <c r="G108" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B109">
         <v>15</v>
@@ -4079,12 +4079,12 @@
         <v>2</v>
       </c>
       <c r="G109" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B110">
         <v>7</v>
@@ -4102,12 +4102,12 @@
         <v>0</v>
       </c>
       <c r="G110" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B111">
         <v>9</v>
@@ -4125,12 +4125,12 @@
         <v>0</v>
       </c>
       <c r="G111" s="2" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B112">
         <v>11</v>
@@ -4148,12 +4148,12 @@
         <v>1</v>
       </c>
       <c r="G112" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B113">
         <v>9</v>
@@ -4171,12 +4171,12 @@
         <v>3</v>
       </c>
       <c r="G113" s="2" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B114">
         <v>7</v>
@@ -4194,12 +4194,12 @@
         <v>2</v>
       </c>
       <c r="G114" s="2" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B115">
         <v>20</v>
@@ -4217,12 +4217,12 @@
         <v>2</v>
       </c>
       <c r="G115" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B116">
         <v>27</v>
@@ -4240,12 +4240,12 @@
         <v>2</v>
       </c>
       <c r="G116" s="2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B117">
         <v>10</v>
@@ -4263,12 +4263,12 @@
         <v>0</v>
       </c>
       <c r="G117" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B118">
         <v>14</v>
@@ -4286,12 +4286,12 @@
         <v>1</v>
       </c>
       <c r="G118" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B119">
         <v>20</v>
@@ -4309,12 +4309,12 @@
         <v>2</v>
       </c>
       <c r="G119" s="2" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B120">
         <v>16</v>
@@ -4332,12 +4332,12 @@
         <v>3</v>
       </c>
       <c r="G120" s="2" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B121">
         <v>0</v>
@@ -4355,12 +4355,12 @@
         <v>2</v>
       </c>
       <c r="G121" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B122">
         <v>0</v>
@@ -4378,12 +4378,12 @@
         <v>3</v>
       </c>
       <c r="G122" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B123">
         <v>6</v>
@@ -4401,12 +4401,12 @@
         <v>0</v>
       </c>
       <c r="G123" s="2" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B124">
         <v>6</v>
@@ -4424,12 +4424,12 @@
         <v>1</v>
       </c>
       <c r="G124" s="2" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B125">
         <v>6</v>
@@ -4447,12 +4447,12 @@
         <v>2</v>
       </c>
       <c r="G125" s="2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B126">
         <v>6</v>
@@ -4470,12 +4470,12 @@
         <v>1</v>
       </c>
       <c r="G126" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B127">
         <v>3</v>
@@ -4493,12 +4493,12 @@
         <v>1</v>
       </c>
       <c r="G127" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B128">
         <v>12</v>
@@ -4516,12 +4516,12 @@
         <v>2</v>
       </c>
       <c r="G128" s="2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B129">
         <v>10</v>
@@ -4539,12 +4539,12 @@
         <v>1</v>
       </c>
       <c r="G129" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B130">
         <v>7</v>
@@ -4562,12 +4562,12 @@
         <v>3</v>
       </c>
       <c r="G130" s="2" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B131">
         <v>4</v>
@@ -4585,12 +4585,12 @@
         <v>2</v>
       </c>
       <c r="G131" s="2" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B132">
         <v>6</v>
@@ -4608,12 +4608,12 @@
         <v>2</v>
       </c>
       <c r="G132" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B133">
         <v>14</v>
@@ -4631,12 +4631,12 @@
         <v>2</v>
       </c>
       <c r="G133" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B134">
         <v>4</v>
@@ -4654,12 +4654,12 @@
         <v>0</v>
       </c>
       <c r="G134" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B135">
         <v>4</v>
@@ -4677,12 +4677,12 @@
         <v>2</v>
       </c>
       <c r="G135" s="2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B136">
         <v>4</v>
@@ -4700,12 +4700,12 @@
         <v>0</v>
       </c>
       <c r="G136" s="2" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B137">
         <v>4</v>
@@ -4723,12 +4723,12 @@
         <v>2</v>
       </c>
       <c r="G137" s="2" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B138">
         <v>4</v>
@@ -4746,12 +4746,12 @@
         <v>1</v>
       </c>
       <c r="G138" s="2" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B139">
         <v>4</v>
@@ -4769,12 +4769,12 @@
         <v>2</v>
       </c>
       <c r="G139" s="2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B140">
         <v>4</v>
@@ -4792,12 +4792,12 @@
         <v>3</v>
       </c>
       <c r="G140" s="2" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B141">
         <v>5</v>
@@ -4815,12 +4815,12 @@
         <v>0</v>
       </c>
       <c r="G141" s="2" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B142">
         <v>6</v>
@@ -4838,12 +4838,12 @@
         <v>0</v>
       </c>
       <c r="G142" s="2" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B143">
         <v>8</v>
@@ -4861,12 +4861,12 @@
         <v>1</v>
       </c>
       <c r="G143" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B144">
         <v>7</v>
@@ -4884,12 +4884,12 @@
         <v>1</v>
       </c>
       <c r="G144" s="2" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B145">
         <v>6</v>
@@ -4907,12 +4907,12 @@
         <v>0</v>
       </c>
       <c r="G145" s="2" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B146">
         <v>6</v>
@@ -4930,12 +4930,12 @@
         <v>1</v>
       </c>
       <c r="G146" s="2" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B147">
         <v>6</v>
@@ -4953,12 +4953,12 @@
         <v>0</v>
       </c>
       <c r="G147" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B148">
         <v>6</v>
@@ -4976,12 +4976,12 @@
         <v>0</v>
       </c>
       <c r="G148" s="2" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B149">
         <v>10</v>
@@ -4999,12 +4999,12 @@
         <v>1</v>
       </c>
       <c r="G149" s="2" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B150">
         <v>7</v>
@@ -5022,12 +5022,12 @@
         <v>0</v>
       </c>
       <c r="G150" s="2" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B151">
         <v>10</v>
@@ -5045,12 +5045,12 @@
         <v>2</v>
       </c>
       <c r="G151" s="2" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B152">
         <v>12</v>
@@ -5068,12 +5068,12 @@
         <v>1</v>
       </c>
       <c r="G152" s="2" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B153">
         <v>6</v>
@@ -5091,12 +5091,12 @@
         <v>0</v>
       </c>
       <c r="G153" s="2" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B154">
         <v>7</v>
@@ -5114,12 +5114,12 @@
         <v>1</v>
       </c>
       <c r="G154" s="2" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B155">
         <v>7</v>
@@ -5137,12 +5137,12 @@
         <v>1</v>
       </c>
       <c r="G155" s="2" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B156">
         <v>8</v>
@@ -5160,12 +5160,12 @@
         <v>1</v>
       </c>
       <c r="G156" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B157">
         <v>10</v>
@@ -5183,12 +5183,12 @@
         <v>1</v>
       </c>
       <c r="G157" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B158">
         <v>10</v>
@@ -5206,12 +5206,12 @@
         <v>2</v>
       </c>
       <c r="G158" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B159">
         <v>10</v>
@@ -5229,12 +5229,12 @@
         <v>2</v>
       </c>
       <c r="G159" s="2" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B160">
         <v>10</v>
@@ -5252,12 +5252,12 @@
         <v>1</v>
       </c>
       <c r="G160" s="2" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B161">
         <v>12</v>
@@ -5275,12 +5275,12 @@
         <v>3</v>
       </c>
       <c r="G161" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B162">
         <v>12</v>
@@ -5298,12 +5298,12 @@
         <v>2</v>
       </c>
       <c r="G162" s="2" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B163">
         <v>14</v>
@@ -5321,12 +5321,12 @@
         <v>3</v>
       </c>
       <c r="G163" s="2" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B164">
         <v>14</v>
@@ -5344,12 +5344,12 @@
         <v>3</v>
       </c>
       <c r="G164" s="2" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B165">
         <v>16</v>
@@ -5367,12 +5367,12 @@
         <v>2</v>
       </c>
       <c r="G165" s="2" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B166">
         <v>11</v>
@@ -5390,12 +5390,12 @@
         <v>2</v>
       </c>
       <c r="G166" s="2" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B167">
         <v>10</v>
@@ -5413,12 +5413,12 @@
         <v>1</v>
       </c>
       <c r="G167" s="2" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B168">
         <v>10</v>
@@ -5436,12 +5436,12 @@
         <v>2</v>
       </c>
       <c r="G168" s="2" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B169">
         <v>10</v>
@@ -5459,12 +5459,12 @@
         <v>2</v>
       </c>
       <c r="G169" s="2" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B170">
         <v>10</v>
@@ -5482,12 +5482,12 @@
         <v>3</v>
       </c>
       <c r="G170" s="2" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B171">
         <v>10</v>
@@ -5505,12 +5505,12 @@
         <v>2</v>
       </c>
       <c r="G171" s="2" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B172">
         <v>10</v>
@@ -5528,12 +5528,12 @@
         <v>2</v>
       </c>
       <c r="G172" s="2" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B173">
         <v>10</v>
@@ -5551,12 +5551,12 @@
         <v>2</v>
       </c>
       <c r="G173" s="2" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B174">
         <v>14</v>
@@ -5574,12 +5574,12 @@
         <v>2</v>
       </c>
       <c r="G174" s="2" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B175">
         <v>30</v>
@@ -5597,12 +5597,12 @@
         <v>1</v>
       </c>
       <c r="G175" s="2" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B176">
         <v>30</v>
@@ -5620,12 +5620,12 @@
         <v>1</v>
       </c>
       <c r="G176" s="2" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B177">
         <v>38</v>
@@ -5643,12 +5643,12 @@
         <v>2</v>
       </c>
       <c r="G177" s="2" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B178">
         <v>16</v>
@@ -5666,12 +5666,12 @@
         <v>2</v>
       </c>
       <c r="G178" s="2" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B179">
         <v>34</v>
@@ -5689,12 +5689,12 @@
         <v>1</v>
       </c>
       <c r="G179" s="2" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B180">
         <v>50</v>
@@ -5712,12 +5712,12 @@
         <v>3</v>
       </c>
       <c r="G180" s="2" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B181">
         <v>34</v>
@@ -5735,12 +5735,12 @@
         <v>3</v>
       </c>
       <c r="G181" s="2" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B182">
         <v>36</v>
@@ -5758,12 +5758,12 @@
         <v>2</v>
       </c>
       <c r="G182" s="2" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B183">
         <v>31</v>
@@ -5781,7 +5781,7 @@
         <v>2</v>
       </c>
       <c r="G183" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
   </sheetData>

</xml_diff>